<commit_message>
third commit - tc_8 and tc_22 issue
</commit_message>
<xml_diff>
--- a/Flatworld_Kohler/folderfolder/Kohler_TestData.xlsx
+++ b/Flatworld_Kohler/folderfolder/Kohler_TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="118">
   <si>
     <t>Tc_Id</t>
   </si>
@@ -373,6 +373,9 @@
   </si>
   <si>
     <t>TestID1511</t>
+  </si>
+  <si>
+    <t>TestID261</t>
   </si>
 </sst>
 </file>
@@ -863,7 +866,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>

</xml_diff>